<commit_message>
add cases about index table truncate and vector join
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/ddl/sql_ddl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/ddl/sql_ddl_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
   <si>
     <t>TestID</t>
   </si>
@@ -256,6 +256,106 @@
   </si>
   <si>
     <t>justExec</t>
+  </si>
+  <si>
+    <t>ddl_011</t>
+  </si>
+  <si>
+    <t>ddl_012</t>
+  </si>
+  <si>
+    <t>清空带有标量和向量索引的单分区空表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_013</t>
+  </si>
+  <si>
+    <t>ddl_014</t>
+  </si>
+  <si>
+    <t>清空带有标量和向量索引的单分区非空表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mixindex015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mix015_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>truncate table $mixindex015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,feature_id1,feature1_index$distance from vector($mixindex015, feature1, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784], 10) where name='' order by feature1_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_011.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name,feature_id2,feature2_index$distance from vector($mixindex015, feature2, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_012.csv</t>
+  </si>
+  <si>
+    <t>清空带有标量和向量索引的多分区空表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空带有标量和向量索引的多分区非空表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mixindex016</t>
+  </si>
+  <si>
+    <t>truncate table $mixindex016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($mixindex016, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_013.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_014.csv</t>
+  </si>
+  <si>
+    <t>mixindex017</t>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,birthday,feature_id,feature_index$distance from vector($mixindex017, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where birthday='2004-12-23' order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>truncate table $mixindex017</t>
+  </si>
+  <si>
+    <t>mix_common_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_015</t>
+  </si>
+  <si>
+    <t>清空带有标量和向量索引的单分区非空表-标量查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_015.csv</t>
+  </si>
+  <si>
+    <t>select id,name from $mixindex015 where name=''</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -625,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -982,6 +1082,175 @@
       </c>
       <c r="K11" s="1" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add case about select constant push down and database/schema ddl
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/ddl/sql_ddl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/ddl/sql_ddl_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="119">
   <si>
     <t>TestID</t>
   </si>
@@ -355,6 +355,97 @@
   </si>
   <si>
     <t>select id,name from $mixindex015 where name=''</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_016</t>
+  </si>
+  <si>
+    <t>创建Database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_017</t>
+  </si>
+  <si>
+    <t>创建Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create database ddl_016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create schema ddl_017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show databases</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show databases like 'ddl_017'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>csv_contains</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_016.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_017.csv</t>
+  </si>
+  <si>
+    <t>ddl_018</t>
+  </si>
+  <si>
+    <t>ddl_019</t>
+  </si>
+  <si>
+    <t>删除database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show databases like 'ddl_018'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show databases like 'ddl_019'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_018.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_019.csv</t>
+  </si>
+  <si>
+    <t>schemaCreate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schemaDrop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create schema ddl_019;drop schema ddl_019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create database ddl_018;drop database ddl_018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>databaseCreate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>databaseDrop</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -424,6 +515,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -725,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1253,6 +1347,122 @@
         <v>25</v>
       </c>
     </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
@@ -1260,7 +1470,7 @@
       <formula1>"y,n"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
-      <formula1>"csv_equals,csv_containsAll,string_equals,effected_rows_assert,table_assert,assertNull,justExec,SQLException"</formula1>
+      <formula1>"csv_equals,csv_containsAll,csv_contains,string_equals,effected_rows_assert,table_assert,schema_assert,assertNull,justExec,SQLException"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add information_schema tables info check
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/ddl/sql_ddl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/ddl/sql_ddl_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="128">
   <si>
     <t>TestID</t>
   </si>
@@ -447,6 +447,39 @@
   <si>
     <t>databaseDrop</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除表后验证是否从information_schema.tables中移除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drop table $schema56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='$schema56' or `TABLE_SCHEMA` in ('MYSQL', 'INFORMATION_SCHEMA')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_020</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/ddl/expectedresult/ddl_020.csv</t>
+  </si>
+  <si>
+    <t>csv_containsAll</t>
   </si>
 </sst>
 </file>
@@ -819,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1461,6 +1494,39 @@
       </c>
       <c r="K20" s="6" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A21" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>